<commit_message>
Investigating Catalan Juvenile Recidivism Data
</commit_message>
<xml_diff>
--- a/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-columns.xlsx
+++ b/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-columns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\DTU\Master_thesis\Fairness-oriented-interpretability-of-predictive-algorithms\data\interim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\DTU\Master_thesis\Fairness-oriented-interpretability-of-predictive-algorithms\data\interim\catalan-juvenile-recidivism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212BE531-F249-4D00-A810-B02385134495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EA3C4A-AA29-49A2-A881-C3FA228AFA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="312">
   <si>
     <t>id</t>
   </si>
@@ -451,9 +451,6 @@
     <t>V132_REINCIDENCIA_2013</t>
   </si>
   <si>
-    <t>Translation</t>
-  </si>
-  <si>
     <t>V1_sex</t>
   </si>
   <si>
@@ -463,36 +460,18 @@
     <t>V3_nationality_country</t>
   </si>
   <si>
-    <t>V4_geographical_area_of_origin</t>
-  </si>
-  <si>
-    <t>V5_age_cat_at_time_of_crime</t>
-  </si>
-  <si>
     <t>V6_province</t>
   </si>
   <si>
     <t>V7_region</t>
   </si>
   <si>
-    <t>V8_age_at_time_of_crime</t>
-  </si>
-  <si>
-    <t>V9_offenders_age_at_program_end</t>
-  </si>
-  <si>
     <t>V10_date_of_birth</t>
   </si>
   <si>
     <t>V11_criminal_record</t>
   </si>
   <si>
-    <t>V14_main_comitted_crime</t>
-  </si>
-  <si>
-    <t>V15_main_comitted_crime_cat</t>
-  </si>
-  <si>
     <t>V16_violent_record</t>
   </si>
   <si>
@@ -502,33 +481,12 @@
     <t>V19_comitted_crime</t>
   </si>
   <si>
-    <t>V20_n_criminal_records_at_juvenile_justice</t>
-  </si>
-  <si>
-    <t>V21_n_crimes</t>
-  </si>
-  <si>
-    <t>V13_n_crimes_cat</t>
-  </si>
-  <si>
-    <t>V12_n_criminal_records_cat</t>
-  </si>
-  <si>
     <t>V22_comission_date_of_main_crime</t>
   </si>
   <si>
     <t>V23_territory_of_execution</t>
   </si>
   <si>
-    <t>V24_finished_program_or_measure</t>
-  </si>
-  <si>
-    <t>V26_finished_measure_cat</t>
-  </si>
-  <si>
-    <t>V25_program_measure_cat</t>
-  </si>
-  <si>
     <t>V27_duration_of_program_cat</t>
   </si>
   <si>
@@ -748,9 +706,6 @@
     <t>V99_SAVRY_MODEL_mean_subsceptibility_of_treatment</t>
   </si>
   <si>
-    <t>V100_RECID2015_n_crimes_in_first_recid</t>
-  </si>
-  <si>
     <t>V101_RECID2015_date_first_recid</t>
   </si>
   <si>
@@ -778,9 +733,6 @@
     <t>V115_RECID2015_recid_bool</t>
   </si>
   <si>
-    <t>V116_RECID2013_n_crimes_first_recid</t>
-  </si>
-  <si>
     <t>V117_RECID2013_date_first_recid</t>
   </si>
   <si>
@@ -845,13 +797,172 @@
   </si>
   <si>
     <t>V132_RECID2013_recid_bool</t>
+  </si>
+  <si>
+    <t>translation</t>
+  </si>
+  <si>
+    <t>V4_area_origin</t>
+  </si>
+  <si>
+    <t>V5_age_cat</t>
+  </si>
+  <si>
+    <t>V8_age</t>
+  </si>
+  <si>
+    <t>V9_age_at_program_end</t>
+  </si>
+  <si>
+    <t>V20_n_juvenile_records</t>
+  </si>
+  <si>
+    <t>V14_main_crime</t>
+  </si>
+  <si>
+    <t>V15_main_crime_cat</t>
+  </si>
+  <si>
+    <t>V12_n_criminal_record_cat</t>
+  </si>
+  <si>
+    <t>V13_n_crime_cat</t>
+  </si>
+  <si>
+    <t>V21_n_crime</t>
+  </si>
+  <si>
+    <t>V100_RECID2015_n_crime_in_first_recid</t>
+  </si>
+  <si>
+    <t>V116_RECID2013_n_crime_first_recid</t>
+  </si>
+  <si>
+    <t>V24_finished_program</t>
+  </si>
+  <si>
+    <t>V26_finished_measure_grouped</t>
+  </si>
+  <si>
+    <t>V25_MRM_ATM_or_enforcement_actions</t>
+  </si>
+  <si>
+    <t>Home/Dona</t>
+  </si>
+  <si>
+    <t>Espanyol/Estranger</t>
+  </si>
+  <si>
+    <t>62 countries</t>
+  </si>
+  <si>
+    <t>14 i 15 anys, 16 I 17 anys, NaN</t>
+  </si>
+  <si>
+    <t>'Lleida', 'Barcelona', 'Girona', 'Tarragona'</t>
+  </si>
+  <si>
+    <t>41 regions</t>
+  </si>
+  <si>
+    <t>Unique Values</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Espanya, Magrib, Centre i Sud Amèrica,  Altres, Europa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have added Espanya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NaNs removed </t>
+  </si>
+  <si>
+    <t>blank when V5 is NaN</t>
+  </si>
+  <si>
+    <t>14,15,16,17, NaN</t>
+  </si>
+  <si>
+    <t>13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 27, 46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Look into 46 </t>
+  </si>
+  <si>
+    <t>'Amb antecedents', 'Sense antecedents'</t>
+  </si>
+  <si>
+    <t>'1 o 2 antecedents', 'De 3 a 5 antecedents', 'Més de 5 antecedents', nan</t>
+  </si>
+  <si>
+    <t>NaN are those without sentences</t>
+  </si>
+  <si>
+    <t>'3 fets o més', '2 fets', '1 fet'</t>
+  </si>
+  <si>
+    <t>69 unique strings</t>
+  </si>
+  <si>
+    <t>'Contra les persones', 'Contra la propietat violent', 'Contra la propietat no violent', 'Altres'</t>
+  </si>
+  <si>
+    <t>Violent, No Violent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delicte, Falta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">23 unique strings </t>
+  </si>
+  <si>
+    <t>all unique</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NaN is zero </t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>16 unique strings (appendix 3)</t>
+  </si>
+  <si>
+    <t>Mesures d'execució, ATM, MRM</t>
+  </si>
+  <si>
+    <t>'Internament', 'LV', 'ATM', 'Altres medi obert', 'PBC', 'MRM'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have added MRM and ATM based on V25 and V24 </t>
+  </si>
+  <si>
+    <t>'Menys de 6 mesos', 'De 6 mesos a 1 any', "Més d'1 any"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">numeric, range 1 to 2390, incl. NaNs </t>
+  </si>
+  <si>
+    <t>numeric, range 0 to 2257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -864,6 +975,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -873,7 +990,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -896,13 +1013,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1207,32 +1347,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B144"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1240,87 +1392,132 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="C4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="C6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+      <c r="C8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="C9" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+      <c r="D10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+      <c r="C12" t="s">
+        <v>288</v>
+      </c>
+      <c r="D12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="C13" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1328,95 +1525,134 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="C15" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+      <c r="C16" t="s">
+        <v>291</v>
+      </c>
+      <c r="D16" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="C17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+      <c r="C18" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+      <c r="C19" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="C20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="C21" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="C22" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+      <c r="C23" t="s">
+        <v>300</v>
+      </c>
+      <c r="D23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+      <c r="C24" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="C25" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1424,79 +1660,109 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+      <c r="C27" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+      <c r="C28" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+      <c r="C29" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+      <c r="C30" t="s">
+        <v>306</v>
+      </c>
+      <c r="D30" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="C31" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="C32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="C33" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="C34" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+      <c r="C35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1504,100 +1770,100 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1605,7 +1871,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1613,7 +1879,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1621,7 +1887,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1629,7 +1895,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1637,7 +1903,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1645,7 +1911,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1653,7 +1919,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1661,7 +1927,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1669,7 +1935,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1685,7 +1951,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1701,7 +1967,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1709,7 +1975,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1717,7 +1983,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1725,7 +1991,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1733,7 +1999,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1741,7 +2007,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1749,7 +2015,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1757,7 +2023,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1765,7 +2031,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1773,7 +2039,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1781,7 +2047,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1797,7 +2063,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1805,7 +2071,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1813,7 +2079,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1821,7 +2087,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1829,7 +2095,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1837,7 +2103,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1845,7 +2111,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1853,7 +2119,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1861,7 +2127,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1869,7 +2135,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1877,7 +2143,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1885,7 +2151,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1893,7 +2159,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1901,7 +2167,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1909,7 +2175,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1917,7 +2183,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1925,7 +2191,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1933,7 +2199,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1941,7 +2207,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1949,7 +2215,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1957,7 +2223,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1965,7 +2231,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1973,7 +2239,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1981,7 +2247,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1997,7 +2263,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -2005,7 +2271,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -2013,7 +2279,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2021,7 +2287,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2029,7 +2295,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -2037,7 +2303,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -2053,7 +2319,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2061,7 +2327,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -2069,7 +2335,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2077,7 +2343,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2085,7 +2351,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -2101,7 +2367,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2109,7 +2375,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -2117,7 +2383,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2125,7 +2391,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -2133,7 +2399,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -2141,7 +2407,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -2149,7 +2415,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -2157,7 +2423,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -2165,7 +2431,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -2173,7 +2439,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -2181,7 +2447,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -2189,7 +2455,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -2197,7 +2463,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -2205,7 +2471,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -2213,7 +2479,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -2221,7 +2487,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -2237,7 +2503,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -2245,7 +2511,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -2253,7 +2519,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -2261,7 +2527,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -2269,7 +2535,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -2277,7 +2543,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -2285,7 +2551,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -2293,7 +2559,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -2301,7 +2567,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -2309,7 +2575,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -2317,7 +2583,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -2325,7 +2591,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -2333,7 +2599,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -2341,7 +2607,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -2349,7 +2615,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
@@ -2357,7 +2623,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -2365,7 +2631,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
folder for models on catalan juvenile recid
</commit_message>
<xml_diff>
--- a/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-columns.xlsx
+++ b/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\DTU\Master_thesis\Fairness-oriented-interpretability-of-predictive-algorithms\data\interim\catalan-juvenile-recidivism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649DA24-BAB0-4A59-9E56-B275383DAB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F3ED11-4CD0-499B-8FD8-599D07390EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding ADNI folder to .gitignore
</commit_message>
<xml_diff>
--- a/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-columns.xlsx
+++ b/data/interim/catalan-juvenile-recidivism/catalan-juvenile-recidivism-columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline\Documents\DTU\Master_thesis\Fairness-oriented-interpretability-of-predictive-algorithms\data\interim\catalan-juvenile-recidivism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F3ED11-4CD0-499B-8FD8-599D07390EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA865F07-6018-4E2B-B096-9A0B737C8770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,9 +943,6 @@
     <t>V27_program_duration_cat</t>
   </si>
   <si>
-    <t>V22_main_crime_comission_date</t>
-  </si>
-  <si>
     <t>V28_days_from_crime_to_program</t>
   </si>
   <si>
@@ -956,6 +953,9 @@
   </si>
   <si>
     <t>V16_violent_crime</t>
+  </si>
+  <si>
+    <t>V22_main_crime_date</t>
   </si>
 </sst>
 </file>
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1620,7 +1620,7 @@
         <v>256</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1628,7 +1628,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C20" t="s">
         <v>284</v>
@@ -1650,7 +1650,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C22" t="s">
         <v>286</v>
@@ -1686,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C25" t="s">
         <v>291</v>
@@ -1763,7 +1763,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
         <v>297</v>

</xml_diff>